<commit_message>
Changed PGOOD LED to 5V rail.
</commit_message>
<xml_diff>
--- a/Fabrication Outputs/BOM.xlsx
+++ b/Fabrication Outputs/BOM.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github projects\Lithium Corporation\BuyDisplay-to-RPi-DSI-adapter\Fabrication Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE4F8A1-27EF-4316-A505-BFA39E640EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A310749-37FF-453D-93BA-A46664CBC37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eagle-export-bom" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'eagle-export-bom'!$A$1:$H$17</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'eagle-export-bom'!$A$1:$H$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -183,9 +182,6 @@
     <t>Analog Devices</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>LED.0603</t>
   </si>
   <si>
@@ -264,23 +260,26 @@
     <t>TMK107BJ105KA8T</t>
   </si>
   <si>
-    <t>Wurth</t>
-  </si>
-  <si>
-    <t>155060SS75300</t>
-  </si>
-  <si>
     <t>Inductor</t>
   </si>
   <si>
     <t>SDR0603-2R5ML</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>LT Q39E-Q1OO-25-1</t>
+  </si>
+  <si>
+    <t>OSRAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,13 +287,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,9 +320,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,17 +396,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF727D4D-D9CD-4572-BE81-CB0544C56D18}" name="eagle_export_bom" displayName="eagle_export_bom" ref="A1:H17" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H17" xr:uid="{DF727D4D-D9CD-4572-BE81-CB0544C56D18}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF727D4D-D9CD-4572-BE81-CB0544C56D18}" name="eagle_export_bom" displayName="eagle_export_bom" ref="A1:H19" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H19" xr:uid="{DF727D4D-D9CD-4572-BE81-CB0544C56D18}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{845DE0BC-D8E0-4E13-9FC5-D0E4DD96028B}" uniqueName="1" name="Qty" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{6FD992C6-D285-4FDA-BC0D-5386BE29E9DE}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{7FEBD130-8AEE-4514-A56C-62613A1A481C}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{A8CFFC93-4EDE-44F6-80FB-74C62382C9E1}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{EDE43DF2-19AB-4D53-9F42-623ED65020AD}" uniqueName="16" name="Manufacturer" queryTableFieldId="16" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{90D12252-D4DF-4868-A7DE-F9C857DDF91D}" uniqueName="15" name="Part Number" queryTableFieldId="15" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{86382CD8-0E9B-4714-8A3B-A0B118644BB7}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{B697A053-78E7-4A7A-989B-97AAFEC2D9D0}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{EDE43DF2-19AB-4D53-9F42-623ED65020AD}" uniqueName="16" name="Manufacturer" queryTableFieldId="16" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{90D12252-D4DF-4868-A7DE-F9C857DDF91D}" uniqueName="15" name="Part Number" queryTableFieldId="15" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{86382CD8-0E9B-4714-8A3B-A0B118644BB7}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B697A053-78E7-4A7A-989B-97AAFEC2D9D0}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942AA0C4-580F-4AE4-81CA-0EA9A6361343}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +707,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -716,10 +733,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -742,10 +759,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>
@@ -768,10 +785,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>
@@ -794,10 +811,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>17</v>
@@ -820,10 +837,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>21</v>
@@ -837,17 +854,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>22</v>
@@ -868,10 +885,10 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
@@ -894,10 +911,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>26</v>
@@ -920,10 +937,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>28</v>
@@ -946,10 +963,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>30</v>
@@ -972,10 +989,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>32</v>
@@ -1061,22 +1078,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>6</v>
@@ -1088,42 +1105,47 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed D1 back to red.
</commit_message>
<xml_diff>
--- a/Fabrication Outputs/BOM.xlsx
+++ b/Fabrication Outputs/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github projects\Lithium Corporation\BuyDisplay-to-RPi-DSI-adapter\Fabrication Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A310749-37FF-453D-93BA-A46664CBC37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136C76D1-1186-4517-AA25-EE44E0DD48DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4035" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t>Qty</t>
   </si>
@@ -266,13 +266,10 @@
     <t>SDR0603-2R5ML</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>LT Q39E-Q1OO-25-1</t>
-  </si>
-  <si>
-    <t>OSRAM</t>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>SML-D12U8WT86C</t>
   </si>
 </sst>
 </file>
@@ -678,7 +675,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1084,7 @@
         <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>77</v>

</xml_diff>